<commit_message>
antes de la bolada
</commit_message>
<xml_diff>
--- a/antivirus/antivirus2.xlsx
+++ b/antivirus/antivirus2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silverit\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silverit\Desktop\goremad-2022\antivirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="891">
   <si>
     <t>INSTALACIÓN DE ANTIVIRUS</t>
   </si>
@@ -2079,6 +2079,630 @@
   </si>
   <si>
     <t>04559-2022</t>
+  </si>
+  <si>
+    <t>172.18.1.115</t>
+  </si>
+  <si>
+    <t>Katia Lucero Huamani Berrocal</t>
+  </si>
+  <si>
+    <t>172.17.1.192</t>
+  </si>
+  <si>
+    <t>Belizabeth Montesinos Dueñas</t>
+  </si>
+  <si>
+    <t>AFEP-11</t>
+  </si>
+  <si>
+    <t>PATRIMONIO-02</t>
+  </si>
+  <si>
+    <t>AFEP-10</t>
+  </si>
+  <si>
+    <t>172.18.1.114</t>
+  </si>
+  <si>
+    <t>Ruth Ñaupa Atamari</t>
+  </si>
+  <si>
+    <t>172.18.1.130</t>
+  </si>
+  <si>
+    <t>Wilfredo F.Gracia Paria</t>
+  </si>
+  <si>
+    <t>AFEP-12</t>
+  </si>
+  <si>
+    <t>172.18.1.111</t>
+  </si>
+  <si>
+    <t>Elmer Rivera Turpo</t>
+  </si>
+  <si>
+    <t>AFEP-13</t>
+  </si>
+  <si>
+    <t>172.18.1.134</t>
+  </si>
+  <si>
+    <t>Adolfo Aestegui Mendes</t>
+  </si>
+  <si>
+    <t>AFEP-14</t>
+  </si>
+  <si>
+    <t>172.18.1.113</t>
+  </si>
+  <si>
+    <t>Diana Corvina Gutierres Mendes</t>
+  </si>
+  <si>
+    <t>AFEP-15</t>
+  </si>
+  <si>
+    <t>172.18.1.96</t>
+  </si>
+  <si>
+    <t>Bryan Arthur Chacacanta Arahujo</t>
+  </si>
+  <si>
+    <t>AFEP-16</t>
+  </si>
+  <si>
+    <t>172.18.1.102</t>
+  </si>
+  <si>
+    <t>Kanly Otsuka Pinche</t>
+  </si>
+  <si>
+    <t>AFEP-17</t>
+  </si>
+  <si>
+    <t>172.18.1.110</t>
+  </si>
+  <si>
+    <t>Javier Edul Tarifa Yucra</t>
+  </si>
+  <si>
+    <t>AFEP-18</t>
+  </si>
+  <si>
+    <t>172.17.1.20</t>
+  </si>
+  <si>
+    <t>Joni Torres Palomino</t>
+  </si>
+  <si>
+    <t>PATRIMONIO-03</t>
+  </si>
+  <si>
+    <t>172.17.1.39</t>
+  </si>
+  <si>
+    <t>Carmen Delgado Alvarado</t>
+  </si>
+  <si>
+    <t>GRI-02</t>
+  </si>
+  <si>
+    <t>172.17.1.133</t>
+  </si>
+  <si>
+    <t>Jackeline Amparo Menacho</t>
+  </si>
+  <si>
+    <t>PATRIMONIO-04</t>
+  </si>
+  <si>
+    <t>Elias Aguirre Huachaca</t>
+  </si>
+  <si>
+    <t>PATRIMONIO-05</t>
+  </si>
+  <si>
+    <t>172.18.1.6</t>
+  </si>
+  <si>
+    <t>OCI-06</t>
+  </si>
+  <si>
+    <t>172.17.1.135</t>
+  </si>
+  <si>
+    <t>Henry Bustinza Acuña</t>
+  </si>
+  <si>
+    <t>PATRIMONIO-06</t>
+  </si>
+  <si>
+    <t>172.17.1.218</t>
+  </si>
+  <si>
+    <t>Jose Guincho</t>
+  </si>
+  <si>
+    <t>PATRIMONIO-07</t>
+  </si>
+  <si>
+    <t>PATRIMONIO-08</t>
+  </si>
+  <si>
+    <t>172.17.1.132</t>
+  </si>
+  <si>
+    <t>172.17.1.35</t>
+  </si>
+  <si>
+    <t>Mishelli Chavez Masias</t>
+  </si>
+  <si>
+    <t>GRI-01</t>
+  </si>
+  <si>
+    <t>18349-2022</t>
+  </si>
+  <si>
+    <t>172.17.1.36</t>
+  </si>
+  <si>
+    <t>Marcos J. Arbieto Flores</t>
+  </si>
+  <si>
+    <t>GRI-03</t>
+  </si>
+  <si>
+    <t>18216-2022</t>
+  </si>
+  <si>
+    <t>Silvia E. Vega</t>
+  </si>
+  <si>
+    <t>GRI-05</t>
+  </si>
+  <si>
+    <t>GRI-06</t>
+  </si>
+  <si>
+    <t>GRI-07</t>
+  </si>
+  <si>
+    <t>GRI-08</t>
+  </si>
+  <si>
+    <t>4152-2022</t>
+  </si>
+  <si>
+    <t>172.17.1.37</t>
+  </si>
+  <si>
+    <t>Miguel A. Gomez Diaz</t>
+  </si>
+  <si>
+    <t>01397-2022</t>
+  </si>
+  <si>
+    <t>172.17.1.34</t>
+  </si>
+  <si>
+    <t>172.17.1.40</t>
+  </si>
+  <si>
+    <t>Roberto Rubin de Celis</t>
+  </si>
+  <si>
+    <t>172.17.1.33</t>
+  </si>
+  <si>
+    <t>Ernesto Victorio Valina</t>
+  </si>
+  <si>
+    <t>Sub Gerencia de Desarrollo
+Institucional e Informatica</t>
+  </si>
+  <si>
+    <t>14948-2022</t>
+  </si>
+  <si>
+    <t>03916-2022</t>
+  </si>
+  <si>
+    <t>172.17.1.16</t>
+  </si>
+  <si>
+    <t>Javier Garcia Blanco</t>
+  </si>
+  <si>
+    <t>SGDIEI-01</t>
+  </si>
+  <si>
+    <t>SGDIEI-02</t>
+  </si>
+  <si>
+    <t>SGDIEI-03</t>
+  </si>
+  <si>
+    <t>03925-2022</t>
+  </si>
+  <si>
+    <t>03932-2022</t>
+  </si>
+  <si>
+    <t>172.17.1.4</t>
+  </si>
+  <si>
+    <t>172.17.1.49</t>
+  </si>
+  <si>
+    <t>Alberto Cruz Valdez</t>
+  </si>
+  <si>
+    <t>Sub Gerencia de Estudio de
+Infraestructura</t>
+  </si>
+  <si>
+    <t>14886-2022</t>
+  </si>
+  <si>
+    <t>172.17.1.55</t>
+  </si>
+  <si>
+    <t>Maricruz Rios Lucana</t>
+  </si>
+  <si>
+    <t>SGEI-01</t>
+  </si>
+  <si>
+    <t>SGEI-02</t>
+  </si>
+  <si>
+    <t>SGEI-03</t>
+  </si>
+  <si>
+    <t>SGEI-04</t>
+  </si>
+  <si>
+    <t>SGEI-05</t>
+  </si>
+  <si>
+    <t>SGEI-06</t>
+  </si>
+  <si>
+    <t>SGEI-07</t>
+  </si>
+  <si>
+    <t>SGEI-08</t>
+  </si>
+  <si>
+    <t>SGEI-09</t>
+  </si>
+  <si>
+    <t>SGEI-10</t>
+  </si>
+  <si>
+    <t>14882-2022</t>
+  </si>
+  <si>
+    <t>14336-2022</t>
+  </si>
+  <si>
+    <t>172.17.1.59</t>
+  </si>
+  <si>
+    <t>Wilson Tarifa Yucra</t>
+  </si>
+  <si>
+    <t>Quispe Caceres</t>
+  </si>
+  <si>
+    <t>Jose Wiliam Villena García</t>
+  </si>
+  <si>
+    <t>Nely Fora Cho</t>
+  </si>
+  <si>
+    <t>Andres Anchopin Nina</t>
+  </si>
+  <si>
+    <t>Waldir Lizereza Cusiyupengi</t>
+  </si>
+  <si>
+    <t>Juan Carlos Chavez</t>
+  </si>
+  <si>
+    <t>Isaac Gongora Pillco</t>
+  </si>
+  <si>
+    <t>Rolando Comarca Figueroa</t>
+  </si>
+  <si>
+    <t>172.17.1.64</t>
+  </si>
+  <si>
+    <t>172.17.1.70</t>
+  </si>
+  <si>
+    <t>172.17.1.50</t>
+  </si>
+  <si>
+    <t>172.17.1.60</t>
+  </si>
+  <si>
+    <t>172.17.1.51</t>
+  </si>
+  <si>
+    <t>172.17.1.52</t>
+  </si>
+  <si>
+    <t>172.17.1.54</t>
+  </si>
+  <si>
+    <t>172.17.1.62</t>
+  </si>
+  <si>
+    <t>14887-2022</t>
+  </si>
+  <si>
+    <t>14885-2022</t>
+  </si>
+  <si>
+    <t>14888-2022</t>
+  </si>
+  <si>
+    <t>14405-2022</t>
+  </si>
+  <si>
+    <t>04181-2022</t>
+  </si>
+  <si>
+    <t>04243-2022</t>
+  </si>
+  <si>
+    <t>14337-2022</t>
+  </si>
+  <si>
+    <t>14889-2022</t>
+  </si>
+  <si>
+    <t>04135-2022</t>
+  </si>
+  <si>
+    <t>14915-2022</t>
+  </si>
+  <si>
+    <t>14404-2022</t>
+  </si>
+  <si>
+    <t>Archivo Tesoreria</t>
+  </si>
+  <si>
+    <t>Archivo Abastecimiento</t>
+  </si>
+  <si>
+    <t>13964-2022</t>
+  </si>
+  <si>
+    <t>00048-2022</t>
+  </si>
+  <si>
+    <t>172.17.1.53</t>
+  </si>
+  <si>
+    <t>Sub Gerencia de Obras</t>
+  </si>
+  <si>
+    <t>19682-2022</t>
+  </si>
+  <si>
+    <t>172.17.1.28</t>
+  </si>
+  <si>
+    <t>Alfredo Tito Rivas</t>
+  </si>
+  <si>
+    <t>Maria Amachi Ramos</t>
+  </si>
+  <si>
+    <t>SGEI-11</t>
+  </si>
+  <si>
+    <t>SGEI-12</t>
+  </si>
+  <si>
+    <t>SGEI-13</t>
+  </si>
+  <si>
+    <t>SGEI-14</t>
+  </si>
+  <si>
+    <t>172.17.1.66</t>
+  </si>
+  <si>
+    <t>172.17.1.57</t>
+  </si>
+  <si>
+    <t>172.17.1.19</t>
+  </si>
+  <si>
+    <t>172.17.1.204</t>
+  </si>
+  <si>
+    <t>172.17.1.209</t>
+  </si>
+  <si>
+    <t>172.17.1.245</t>
+  </si>
+  <si>
+    <t>172.17.1.32</t>
+  </si>
+  <si>
+    <t>07151-2022</t>
+  </si>
+  <si>
+    <t>14722-2022</t>
+  </si>
+  <si>
+    <t>17561-2022</t>
+  </si>
+  <si>
+    <t>18195-2022</t>
+  </si>
+  <si>
+    <t>02040-2022</t>
+  </si>
+  <si>
+    <t>17748-2022</t>
+  </si>
+  <si>
+    <t>01950-2022</t>
+  </si>
+  <si>
+    <t>07953-2022</t>
+  </si>
+  <si>
+    <t>00418-2022</t>
+  </si>
+  <si>
+    <t>17438-2022</t>
+  </si>
+  <si>
+    <t>13514-2022</t>
+  </si>
+  <si>
+    <t>13515-2022</t>
+  </si>
+  <si>
+    <t>14229-2022</t>
+  </si>
+  <si>
+    <t>01929-2022</t>
+  </si>
+  <si>
+    <t>Miguel Santa Valdes</t>
+  </si>
+  <si>
+    <t>Clara Casanova Victoriano</t>
+  </si>
+  <si>
+    <t>Silvia Rocio Ccapo Cruz</t>
+  </si>
+  <si>
+    <t>Santos Imayo Cortes</t>
+  </si>
+  <si>
+    <t>Lilian Choquemamani Vera</t>
+  </si>
+  <si>
+    <t>Clara Antonieta Torres</t>
+  </si>
+  <si>
+    <t>Eduardo Ojeda Rosas</t>
+  </si>
+  <si>
+    <t>AT-01</t>
+  </si>
+  <si>
+    <t>SGO-03</t>
+  </si>
+  <si>
+    <t>SGO-04</t>
+  </si>
+  <si>
+    <t>SGO-05</t>
+  </si>
+  <si>
+    <t>SGO-06</t>
+  </si>
+  <si>
+    <t>SGO-07</t>
+  </si>
+  <si>
+    <t>ARCHIVO
+ABASTECIMIENTO-01</t>
+  </si>
+  <si>
+    <t>SGO-01</t>
+  </si>
+  <si>
+    <t>SGO-02</t>
+  </si>
+  <si>
+    <t>SGO-08</t>
+  </si>
+  <si>
+    <t>SGO-09</t>
+  </si>
+  <si>
+    <t>SGO-10</t>
+  </si>
+  <si>
+    <t>SGO-11</t>
+  </si>
+  <si>
+    <t>SGO-12</t>
+  </si>
+  <si>
+    <t>SGO-13</t>
+  </si>
+  <si>
+    <t>SGO-14</t>
+  </si>
+  <si>
+    <t>SGO-15</t>
+  </si>
+  <si>
+    <t>172.17.1.116</t>
+  </si>
+  <si>
+    <t>172.17.1.173</t>
+  </si>
+  <si>
+    <t>172.17.1.42</t>
+  </si>
+  <si>
+    <t>172.17.1.169</t>
+  </si>
+  <si>
+    <t>172.17.1.162</t>
+  </si>
+  <si>
+    <t>172.17.1.170</t>
+  </si>
+  <si>
+    <t>172.17.1.171</t>
+  </si>
+  <si>
+    <t>172.17.1.163</t>
+  </si>
+  <si>
+    <t>172.17.1.165</t>
+  </si>
+  <si>
+    <t>172.17.1.175</t>
+  </si>
+  <si>
+    <t>172.17.1.220</t>
+  </si>
+  <si>
+    <t>Sonia Maceda Guerra</t>
+  </si>
+  <si>
+    <t>Gisela Yuana Grifa</t>
+  </si>
+  <si>
+    <t>Angie Camera Herrera</t>
+  </si>
+  <si>
+    <t>Lidiany Lopez Gongora</t>
+  </si>
+  <si>
+    <t>Alessandra Georgina León</t>
+  </si>
+  <si>
+    <t>Rossmery Vanessa</t>
   </si>
 </sst>
 </file>
@@ -2119,7 +2743,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -2375,11 +2999,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2452,6 +3087,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2737,10 +3378,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H220"/>
+  <dimension ref="A1:H222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="D161" sqref="D161"/>
+    <sheetView tabSelected="1" topLeftCell="A204" workbookViewId="0">
+      <selection activeCell="F214" sqref="F214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6367,27 +7008,27 @@
       </c>
       <c r="H151" s="7"/>
     </row>
-    <row r="152" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="9">
         <v>150</v>
       </c>
-      <c r="B152" s="16" t="s">
-        <v>616</v>
-      </c>
-      <c r="C152" s="16" t="s">
-        <v>629</v>
-      </c>
-      <c r="D152" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E152" s="16" t="s">
-        <v>627</v>
-      </c>
-      <c r="F152" s="16" t="s">
-        <v>628</v>
-      </c>
-      <c r="G152" s="16" t="s">
-        <v>639</v>
+      <c r="B152" s="24" t="s">
+        <v>585</v>
+      </c>
+      <c r="C152" s="24" t="s">
+        <v>670</v>
+      </c>
+      <c r="D152" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E152" s="24" t="s">
+        <v>725</v>
+      </c>
+      <c r="F152" s="24" t="s">
+        <v>598</v>
+      </c>
+      <c r="G152" s="24" t="s">
+        <v>726</v>
       </c>
       <c r="H152" s="7"/>
     </row>
@@ -6399,19 +7040,19 @@
         <v>616</v>
       </c>
       <c r="C153" s="16" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D153" s="16" t="s">
         <v>11</v>
       </c>
       <c r="E153" s="16" t="s">
-        <v>649</v>
+        <v>627</v>
       </c>
       <c r="F153" s="16" t="s">
-        <v>657</v>
+        <v>628</v>
       </c>
       <c r="G153" s="16" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="H153" s="7"/>
     </row>
@@ -6447,19 +7088,19 @@
         <v>616</v>
       </c>
       <c r="C155" s="16" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="D155" s="16" t="s">
         <v>11</v>
       </c>
       <c r="E155" s="16" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="F155" s="16" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="G155" s="16" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="H155" s="7"/>
     </row>
@@ -6471,19 +7112,19 @@
         <v>616</v>
       </c>
       <c r="C156" s="16" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D156" s="16" t="s">
         <v>11</v>
       </c>
       <c r="E156" s="16" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="F156" s="16" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="G156" s="16" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="H156" s="7"/>
     </row>
@@ -6494,20 +7135,20 @@
       <c r="B157" s="16" t="s">
         <v>616</v>
       </c>
-      <c r="C157" s="19" t="s">
-        <v>634</v>
-      </c>
-      <c r="D157" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E157" s="19" t="s">
-        <v>653</v>
-      </c>
-      <c r="F157" s="19" t="s">
-        <v>661</v>
+      <c r="C157" s="16" t="s">
+        <v>633</v>
+      </c>
+      <c r="D157" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E157" s="16" t="s">
+        <v>652</v>
+      </c>
+      <c r="F157" s="16" t="s">
+        <v>660</v>
       </c>
       <c r="G157" s="16" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="H157" s="11"/>
     </row>
@@ -6518,44 +7159,44 @@
       <c r="B158" s="16" t="s">
         <v>616</v>
       </c>
-      <c r="C158" s="21" t="s">
-        <v>635</v>
-      </c>
-      <c r="D158" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E158" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="F158" s="21" t="s">
-        <v>662</v>
+      <c r="C158" s="19" t="s">
+        <v>634</v>
+      </c>
+      <c r="D158" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E158" s="19" t="s">
+        <v>653</v>
+      </c>
+      <c r="F158" s="19" t="s">
+        <v>661</v>
       </c>
       <c r="G158" s="16" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="H158" s="15"/>
     </row>
-    <row r="159" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="9">
         <v>157</v>
       </c>
       <c r="B159" s="16" t="s">
         <v>616</v>
       </c>
-      <c r="C159" s="22" t="s">
-        <v>636</v>
-      </c>
-      <c r="D159" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E159" s="22" t="s">
-        <v>654</v>
-      </c>
-      <c r="F159" s="22" t="s">
-        <v>663</v>
+      <c r="C159" s="21" t="s">
+        <v>635</v>
+      </c>
+      <c r="D159" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E159" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="F159" s="21" t="s">
+        <v>662</v>
       </c>
       <c r="G159" s="16" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="H159" s="14"/>
     </row>
@@ -6566,20 +7207,20 @@
       <c r="B160" s="16" t="s">
         <v>616</v>
       </c>
-      <c r="C160" s="16" t="s">
-        <v>637</v>
-      </c>
-      <c r="D160" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E160" s="16" t="s">
-        <v>655</v>
-      </c>
-      <c r="F160" s="16" t="s">
-        <v>664</v>
+      <c r="C160" s="22" t="s">
+        <v>636</v>
+      </c>
+      <c r="D160" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E160" s="22" t="s">
+        <v>654</v>
+      </c>
+      <c r="F160" s="22" t="s">
+        <v>663</v>
       </c>
       <c r="G160" s="16" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="H160" s="7"/>
     </row>
@@ -6588,22 +7229,22 @@
         <v>159</v>
       </c>
       <c r="B161" s="16" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C161" s="16" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D161" s="16" t="s">
         <v>11</v>
       </c>
       <c r="E161" s="16" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="F161" s="16" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="G161" s="16" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="H161" s="7"/>
     </row>
@@ -6612,15 +7253,23 @@
         <v>160</v>
       </c>
       <c r="B162" s="16" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C162" s="16" t="s">
-        <v>675</v>
-      </c>
-      <c r="D162" s="16"/>
-      <c r="E162" s="16"/>
-      <c r="F162" s="16"/>
-      <c r="G162" s="16"/>
+        <v>676</v>
+      </c>
+      <c r="D162" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E162" s="16" t="s">
+        <v>684</v>
+      </c>
+      <c r="F162" s="16" t="s">
+        <v>685</v>
+      </c>
+      <c r="G162" s="16" t="s">
+        <v>690</v>
+      </c>
       <c r="H162" s="7"/>
     </row>
     <row r="163" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6631,12 +7280,20 @@
         <v>616</v>
       </c>
       <c r="C163" s="16" t="s">
-        <v>676</v>
-      </c>
-      <c r="D163" s="16"/>
-      <c r="E163" s="16"/>
-      <c r="F163" s="16"/>
-      <c r="G163" s="16"/>
+        <v>677</v>
+      </c>
+      <c r="D163" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E163" s="16" t="s">
+        <v>691</v>
+      </c>
+      <c r="F163" s="16" t="s">
+        <v>692</v>
+      </c>
+      <c r="G163" s="16" t="s">
+        <v>688</v>
+      </c>
       <c r="H163" s="7"/>
     </row>
     <row r="164" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6647,12 +7304,20 @@
         <v>616</v>
       </c>
       <c r="C164" s="16" t="s">
-        <v>677</v>
-      </c>
-      <c r="D164" s="16"/>
-      <c r="E164" s="16"/>
-      <c r="F164" s="16"/>
-      <c r="G164" s="16"/>
+        <v>678</v>
+      </c>
+      <c r="D164" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E164" s="16" t="s">
+        <v>693</v>
+      </c>
+      <c r="F164" s="16" t="s">
+        <v>694</v>
+      </c>
+      <c r="G164" s="16" t="s">
+        <v>695</v>
+      </c>
       <c r="H164" s="7"/>
     </row>
     <row r="165" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6663,12 +7328,20 @@
         <v>616</v>
       </c>
       <c r="C165" s="16" t="s">
-        <v>678</v>
-      </c>
-      <c r="D165" s="16"/>
-      <c r="E165" s="16"/>
-      <c r="F165" s="16"/>
-      <c r="G165" s="16"/>
+        <v>679</v>
+      </c>
+      <c r="D165" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E165" s="16" t="s">
+        <v>696</v>
+      </c>
+      <c r="F165" s="16" t="s">
+        <v>697</v>
+      </c>
+      <c r="G165" s="16" t="s">
+        <v>698</v>
+      </c>
       <c r="H165" s="7"/>
     </row>
     <row r="166" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6679,12 +7352,20 @@
         <v>616</v>
       </c>
       <c r="C166" s="16" t="s">
-        <v>679</v>
-      </c>
-      <c r="D166" s="16"/>
-      <c r="E166" s="16"/>
-      <c r="F166" s="16"/>
-      <c r="G166" s="16"/>
+        <v>680</v>
+      </c>
+      <c r="D166" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E166" s="16" t="s">
+        <v>699</v>
+      </c>
+      <c r="F166" s="16" t="s">
+        <v>700</v>
+      </c>
+      <c r="G166" s="16" t="s">
+        <v>701</v>
+      </c>
       <c r="H166" s="7"/>
     </row>
     <row r="167" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6695,28 +7376,44 @@
         <v>616</v>
       </c>
       <c r="C167" s="16" t="s">
-        <v>680</v>
-      </c>
-      <c r="D167" s="16"/>
-      <c r="E167" s="16"/>
-      <c r="F167" s="16"/>
-      <c r="G167" s="16"/>
+        <v>681</v>
+      </c>
+      <c r="D167" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E167" s="16" t="s">
+        <v>702</v>
+      </c>
+      <c r="F167" s="16" t="s">
+        <v>703</v>
+      </c>
+      <c r="G167" s="16" t="s">
+        <v>704</v>
+      </c>
       <c r="H167" s="7"/>
     </row>
-    <row r="168" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="9">
         <v>166</v>
       </c>
       <c r="B168" s="16" t="s">
         <v>616</v>
       </c>
-      <c r="C168" s="16" t="s">
-        <v>681</v>
-      </c>
-      <c r="D168" s="16"/>
-      <c r="E168" s="16"/>
-      <c r="F168" s="16"/>
-      <c r="G168" s="16"/>
+      <c r="C168" s="24" t="s">
+        <v>682</v>
+      </c>
+      <c r="D168" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E168" s="24" t="s">
+        <v>705</v>
+      </c>
+      <c r="F168" s="24" t="s">
+        <v>706</v>
+      </c>
+      <c r="G168" s="24" t="s">
+        <v>707</v>
+      </c>
       <c r="H168" s="7"/>
     </row>
     <row r="169" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6727,12 +7424,20 @@
         <v>616</v>
       </c>
       <c r="C169" s="24" t="s">
-        <v>682</v>
-      </c>
-      <c r="D169" s="24"/>
-      <c r="E169" s="24"/>
-      <c r="F169" s="24"/>
-      <c r="G169" s="24"/>
+        <v>683</v>
+      </c>
+      <c r="D169" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E169" s="24" t="s">
+        <v>708</v>
+      </c>
+      <c r="F169" s="24" t="s">
+        <v>709</v>
+      </c>
+      <c r="G169" s="24" t="s">
+        <v>710</v>
+      </c>
       <c r="H169" s="8"/>
     </row>
     <row r="170" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6742,13 +7447,21 @@
       <c r="B170" s="16" t="s">
         <v>616</v>
       </c>
-      <c r="C170" s="24" t="s">
-        <v>683</v>
-      </c>
-      <c r="D170" s="24"/>
-      <c r="E170" s="24"/>
-      <c r="F170" s="24"/>
-      <c r="G170" s="24"/>
+      <c r="C170" s="24">
+        <v>12736</v>
+      </c>
+      <c r="D170" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E170" s="24" t="s">
+        <v>711</v>
+      </c>
+      <c r="F170" s="24" t="s">
+        <v>712</v>
+      </c>
+      <c r="G170" s="24" t="s">
+        <v>713</v>
+      </c>
       <c r="H170" s="8"/>
     </row>
     <row r="171" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6756,45 +7469,71 @@
         <v>169</v>
       </c>
       <c r="B171" s="16" t="s">
-        <v>616</v>
-      </c>
-      <c r="C171" s="24"/>
-      <c r="D171" s="24"/>
-      <c r="E171" s="24"/>
-      <c r="F171" s="24"/>
-      <c r="G171" s="24"/>
+        <v>617</v>
+      </c>
+      <c r="C171" s="16" t="s">
+        <v>638</v>
+      </c>
+      <c r="D171" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E171" s="16" t="s">
+        <v>656</v>
+      </c>
+      <c r="F171" s="16" t="s">
+        <v>665</v>
+      </c>
+      <c r="G171" s="16" t="s">
+        <v>648</v>
+      </c>
       <c r="H171" s="8"/>
     </row>
     <row r="172" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="9">
         <v>170</v>
       </c>
-      <c r="B172" s="24" t="s">
+      <c r="B172" s="16" t="s">
         <v>617</v>
       </c>
-      <c r="C172" s="24" t="s">
-        <v>674</v>
-      </c>
-      <c r="D172" s="24"/>
-      <c r="E172" s="24"/>
-      <c r="F172" s="24"/>
-      <c r="G172" s="24"/>
+      <c r="C172" s="16" t="s">
+        <v>675</v>
+      </c>
+      <c r="D172" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E172" s="16" t="s">
+        <v>686</v>
+      </c>
+      <c r="F172" s="23" t="s">
+        <v>687</v>
+      </c>
+      <c r="G172" s="16" t="s">
+        <v>689</v>
+      </c>
       <c r="H172" s="8"/>
     </row>
     <row r="173" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="9">
         <v>171</v>
       </c>
-      <c r="B173" s="26" t="s">
-        <v>666</v>
+      <c r="B173" s="24" t="s">
+        <v>617</v>
       </c>
       <c r="C173" s="24" t="s">
-        <v>673</v>
-      </c>
-      <c r="D173" s="24"/>
-      <c r="E173" s="24"/>
-      <c r="F173" s="24"/>
-      <c r="G173" s="24"/>
+        <v>674</v>
+      </c>
+      <c r="D173" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E173" s="24" t="s">
+        <v>714</v>
+      </c>
+      <c r="F173" s="24" t="s">
+        <v>715</v>
+      </c>
+      <c r="G173" s="24" t="s">
+        <v>716</v>
+      </c>
       <c r="H173" s="8"/>
     </row>
     <row r="174" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6807,10 +7546,18 @@
       <c r="C174" s="24" t="s">
         <v>672</v>
       </c>
-      <c r="D174" s="24"/>
-      <c r="E174" s="24"/>
-      <c r="F174" s="24"/>
-      <c r="G174" s="24"/>
+      <c r="D174" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E174" s="24" t="s">
+        <v>720</v>
+      </c>
+      <c r="F174" s="24" t="s">
+        <v>721</v>
+      </c>
+      <c r="G174" s="24" t="s">
+        <v>722</v>
+      </c>
       <c r="H174" s="8"/>
     </row>
     <row r="175" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6823,10 +7570,18 @@
       <c r="C175" s="24" t="s">
         <v>671</v>
       </c>
-      <c r="D175" s="24"/>
-      <c r="E175" s="24"/>
-      <c r="F175" s="24"/>
-      <c r="G175" s="24"/>
+      <c r="D175" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E175" s="24" t="s">
+        <v>699</v>
+      </c>
+      <c r="F175" s="24" t="s">
+        <v>723</v>
+      </c>
+      <c r="G175" s="24" t="s">
+        <v>724</v>
+      </c>
       <c r="H175" s="8"/>
     </row>
     <row r="176" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6834,15 +7589,23 @@
         <v>174</v>
       </c>
       <c r="B176" s="24" t="s">
-        <v>585</v>
+        <v>617</v>
       </c>
       <c r="C176" s="24" t="s">
-        <v>670</v>
-      </c>
-      <c r="D176" s="24"/>
-      <c r="E176" s="24"/>
-      <c r="F176" s="24"/>
-      <c r="G176" s="24"/>
+        <v>669</v>
+      </c>
+      <c r="D176" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E176" s="24" t="s">
+        <v>727</v>
+      </c>
+      <c r="F176" s="24" t="s">
+        <v>728</v>
+      </c>
+      <c r="G176" s="24" t="s">
+        <v>729</v>
+      </c>
       <c r="H176" s="8"/>
     </row>
     <row r="177" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6853,12 +7616,20 @@
         <v>617</v>
       </c>
       <c r="C177" s="24" t="s">
-        <v>669</v>
-      </c>
-      <c r="D177" s="24"/>
-      <c r="E177" s="24"/>
-      <c r="F177" s="24"/>
-      <c r="G177" s="24"/>
+        <v>150</v>
+      </c>
+      <c r="D177" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E177" s="24" t="s">
+        <v>730</v>
+      </c>
+      <c r="F177" s="24" t="s">
+        <v>731</v>
+      </c>
+      <c r="G177" s="24" t="s">
+        <v>732</v>
+      </c>
       <c r="H177" s="8"/>
     </row>
     <row r="178" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6869,28 +7640,44 @@
         <v>617</v>
       </c>
       <c r="C178" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="D178" s="24"/>
-      <c r="E178" s="24"/>
-      <c r="F178" s="24"/>
-      <c r="G178" s="24"/>
+        <v>668</v>
+      </c>
+      <c r="D178" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E178" s="24" t="s">
+        <v>734</v>
+      </c>
+      <c r="F178" s="24" t="s">
+        <v>715</v>
+      </c>
+      <c r="G178" s="24" t="s">
+        <v>733</v>
+      </c>
       <c r="H178" s="8"/>
     </row>
     <row r="179" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="9">
         <v>177</v>
       </c>
-      <c r="B179" s="24" t="s">
-        <v>617</v>
+      <c r="B179" s="26" t="s">
+        <v>666</v>
       </c>
       <c r="C179" s="24" t="s">
-        <v>668</v>
-      </c>
-      <c r="D179" s="24"/>
-      <c r="E179" s="24"/>
-      <c r="F179" s="24"/>
-      <c r="G179" s="24"/>
+        <v>667</v>
+      </c>
+      <c r="D179" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E179" s="24" t="s">
+        <v>735</v>
+      </c>
+      <c r="F179" s="24" t="s">
+        <v>736</v>
+      </c>
+      <c r="G179" s="24" t="s">
+        <v>737</v>
+      </c>
       <c r="H179" s="8"/>
     </row>
     <row r="180" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6901,493 +7688,969 @@
         <v>666</v>
       </c>
       <c r="C180" s="24" t="s">
-        <v>667</v>
-      </c>
-      <c r="D180" s="24"/>
-      <c r="E180" s="24"/>
-      <c r="F180" s="24"/>
-      <c r="G180" s="24"/>
+        <v>673</v>
+      </c>
+      <c r="D180" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E180" s="24" t="s">
+        <v>717</v>
+      </c>
+      <c r="F180" s="24" t="s">
+        <v>718</v>
+      </c>
+      <c r="G180" s="24" t="s">
+        <v>719</v>
+      </c>
       <c r="H180" s="8"/>
     </row>
     <row r="181" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="9">
         <v>179</v>
       </c>
-      <c r="B181" s="24"/>
-      <c r="C181" s="24"/>
-      <c r="D181" s="24"/>
-      <c r="E181" s="24"/>
-      <c r="F181" s="24"/>
-      <c r="G181" s="24"/>
+      <c r="B181" s="30" t="s">
+        <v>666</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="D181" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E181" s="2" t="s">
+        <v>739</v>
+      </c>
+      <c r="F181" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="G181" s="2" t="s">
+        <v>741</v>
+      </c>
       <c r="H181" s="8"/>
     </row>
     <row r="182" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="9">
         <v>180</v>
       </c>
-      <c r="B182" s="24"/>
-      <c r="C182" s="24"/>
-      <c r="D182" s="24"/>
-      <c r="E182" s="24"/>
-      <c r="F182" s="24"/>
-      <c r="G182" s="24"/>
+      <c r="B182" s="30" t="s">
+        <v>666</v>
+      </c>
+      <c r="C182" s="24" t="s">
+        <v>742</v>
+      </c>
+      <c r="D182" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E182" s="24" t="s">
+        <v>749</v>
+      </c>
+      <c r="F182" s="24" t="s">
+        <v>743</v>
+      </c>
+      <c r="G182" s="24" t="s">
+        <v>744</v>
+      </c>
       <c r="H182" s="8"/>
     </row>
     <row r="183" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="9">
-        <v>17</v>
-      </c>
-      <c r="B183" s="24"/>
-      <c r="C183" s="24"/>
-      <c r="D183" s="24"/>
-      <c r="E183" s="24"/>
-      <c r="F183" s="24"/>
-      <c r="G183" s="24"/>
+        <v>181</v>
+      </c>
+      <c r="B183" s="30" t="s">
+        <v>666</v>
+      </c>
+      <c r="C183" s="24" t="s">
+        <v>748</v>
+      </c>
+      <c r="D183" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E183" s="24" t="s">
+        <v>753</v>
+      </c>
+      <c r="F183" s="24" t="s">
+        <v>750</v>
+      </c>
+      <c r="G183" s="24" t="s">
+        <v>745</v>
+      </c>
       <c r="H183" s="8"/>
     </row>
     <row r="184" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A184" s="9">
-        <v>17</v>
-      </c>
-      <c r="B184" s="24"/>
-      <c r="C184" s="24"/>
-      <c r="D184" s="24"/>
-      <c r="E184" s="24"/>
-      <c r="F184" s="24"/>
-      <c r="G184" s="24"/>
+      <c r="A184" s="31">
+        <v>182</v>
+      </c>
+      <c r="B184" s="30" t="s">
+        <v>666</v>
+      </c>
+      <c r="C184" s="24" t="s">
+        <v>751</v>
+      </c>
+      <c r="D184" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E184" s="24" t="s">
+        <v>752</v>
+      </c>
+      <c r="F184" s="24" t="s">
+        <v>754</v>
+      </c>
+      <c r="G184" s="24" t="s">
+        <v>746</v>
+      </c>
       <c r="H184" s="8"/>
     </row>
     <row r="185" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="9">
-        <v>14</v>
-      </c>
-      <c r="B185" s="24"/>
-      <c r="C185" s="24"/>
-      <c r="D185" s="24"/>
-      <c r="E185" s="24"/>
-      <c r="F185" s="24"/>
-      <c r="G185" s="24"/>
+        <v>183</v>
+      </c>
+      <c r="B185" s="30" t="s">
+        <v>666</v>
+      </c>
+      <c r="C185" s="24" t="s">
+        <v>758</v>
+      </c>
+      <c r="D185" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E185" s="24" t="s">
+        <v>755</v>
+      </c>
+      <c r="F185" s="24" t="s">
+        <v>756</v>
+      </c>
+      <c r="G185" s="24" t="s">
+        <v>747</v>
+      </c>
       <c r="H185" s="8"/>
     </row>
     <row r="186" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="9">
-        <v>14</v>
-      </c>
-      <c r="B186" s="24"/>
-      <c r="C186" s="24"/>
-      <c r="D186" s="24"/>
-      <c r="E186" s="24"/>
-      <c r="F186" s="24"/>
-      <c r="G186" s="24"/>
+        <v>184</v>
+      </c>
+      <c r="B186" s="26" t="s">
+        <v>757</v>
+      </c>
+      <c r="C186" s="24" t="s">
+        <v>759</v>
+      </c>
+      <c r="D186" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E186" s="24" t="s">
+        <v>760</v>
+      </c>
+      <c r="F186" s="24" t="s">
+        <v>761</v>
+      </c>
+      <c r="G186" s="24" t="s">
+        <v>762</v>
+      </c>
       <c r="H186" s="8"/>
     </row>
     <row r="187" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="9">
-        <v>14</v>
-      </c>
-      <c r="B187" s="24"/>
-      <c r="C187" s="24"/>
-      <c r="D187" s="24"/>
-      <c r="E187" s="24"/>
-      <c r="F187" s="24"/>
-      <c r="G187" s="24"/>
+        <v>185</v>
+      </c>
+      <c r="B187" s="26" t="s">
+        <v>757</v>
+      </c>
+      <c r="C187" s="24" t="s">
+        <v>765</v>
+      </c>
+      <c r="D187" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E187" s="24" t="s">
+        <v>767</v>
+      </c>
+      <c r="F187" s="24" t="s">
+        <v>769</v>
+      </c>
+      <c r="G187" s="24" t="s">
+        <v>763</v>
+      </c>
       <c r="H187" s="8"/>
     </row>
     <row r="188" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="9">
-        <v>14</v>
-      </c>
-      <c r="B188" s="24"/>
-      <c r="C188" s="24"/>
-      <c r="D188" s="24"/>
-      <c r="E188" s="24"/>
-      <c r="F188" s="24"/>
-      <c r="G188" s="24"/>
+        <v>186</v>
+      </c>
+      <c r="B188" s="26" t="s">
+        <v>757</v>
+      </c>
+      <c r="C188" s="24" t="s">
+        <v>766</v>
+      </c>
+      <c r="D188" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E188" s="24" t="s">
+        <v>768</v>
+      </c>
+      <c r="F188" s="24" t="s">
+        <v>769</v>
+      </c>
+      <c r="G188" s="24" t="s">
+        <v>764</v>
+      </c>
       <c r="H188" s="8"/>
     </row>
     <row r="189" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="9">
-        <v>14</v>
-      </c>
-      <c r="B189" s="24"/>
-      <c r="C189" s="24"/>
-      <c r="D189" s="24"/>
-      <c r="E189" s="24"/>
-      <c r="F189" s="24"/>
-      <c r="G189" s="24"/>
+        <v>187</v>
+      </c>
+      <c r="B189" s="26" t="s">
+        <v>770</v>
+      </c>
+      <c r="C189" s="24" t="s">
+        <v>771</v>
+      </c>
+      <c r="D189" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E189" s="24" t="s">
+        <v>772</v>
+      </c>
+      <c r="F189" s="24" t="s">
+        <v>773</v>
+      </c>
+      <c r="G189" s="24" t="s">
+        <v>774</v>
+      </c>
       <c r="H189" s="8"/>
     </row>
     <row r="190" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="9">
-        <v>14</v>
-      </c>
-      <c r="B190" s="24"/>
-      <c r="C190" s="24"/>
-      <c r="D190" s="24"/>
-      <c r="E190" s="24"/>
-      <c r="F190" s="24"/>
-      <c r="G190" s="24"/>
+        <v>188</v>
+      </c>
+      <c r="B190" s="26" t="s">
+        <v>770</v>
+      </c>
+      <c r="C190" s="24" t="s">
+        <v>784</v>
+      </c>
+      <c r="D190" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E190" s="24" t="s">
+        <v>786</v>
+      </c>
+      <c r="F190" s="24" t="s">
+        <v>787</v>
+      </c>
+      <c r="G190" s="24" t="s">
+        <v>775</v>
+      </c>
       <c r="H190" s="8"/>
     </row>
     <row r="191" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="9">
-        <v>14</v>
-      </c>
-      <c r="B191" s="24"/>
-      <c r="C191" s="24"/>
-      <c r="D191" s="24"/>
-      <c r="E191" s="24"/>
-      <c r="F191" s="24"/>
-      <c r="G191" s="24"/>
+        <v>189</v>
+      </c>
+      <c r="B191" s="26" t="s">
+        <v>770</v>
+      </c>
+      <c r="C191" s="24" t="s">
+        <v>785</v>
+      </c>
+      <c r="D191" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E191" s="24" t="s">
+        <v>803</v>
+      </c>
+      <c r="F191" s="24" t="s">
+        <v>788</v>
+      </c>
+      <c r="G191" s="24" t="s">
+        <v>776</v>
+      </c>
       <c r="H191" s="8"/>
     </row>
     <row r="192" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="9">
-        <v>14</v>
-      </c>
-      <c r="B192" s="24"/>
-      <c r="C192" s="24"/>
-      <c r="D192" s="24"/>
-      <c r="E192" s="24"/>
-      <c r="F192" s="24"/>
-      <c r="G192" s="24"/>
+        <v>190</v>
+      </c>
+      <c r="B192" s="26" t="s">
+        <v>770</v>
+      </c>
+      <c r="C192" s="24" t="s">
+        <v>804</v>
+      </c>
+      <c r="D192" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E192" s="24" t="s">
+        <v>802</v>
+      </c>
+      <c r="F192" s="24" t="s">
+        <v>789</v>
+      </c>
+      <c r="G192" s="24" t="s">
+        <v>777</v>
+      </c>
       <c r="H192" s="8"/>
     </row>
     <row r="193" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="9">
-        <v>14</v>
-      </c>
-      <c r="B193" s="24"/>
-      <c r="C193" s="24"/>
-      <c r="D193" s="24"/>
-      <c r="E193" s="24"/>
-      <c r="F193" s="24"/>
-      <c r="G193" s="24"/>
+        <v>191</v>
+      </c>
+      <c r="B193" s="26" t="s">
+        <v>770</v>
+      </c>
+      <c r="C193" s="24" t="s">
+        <v>805</v>
+      </c>
+      <c r="D193" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E193" s="24" t="s">
+        <v>801</v>
+      </c>
+      <c r="F193" s="24" t="s">
+        <v>790</v>
+      </c>
+      <c r="G193" s="24" t="s">
+        <v>778</v>
+      </c>
       <c r="H193" s="8"/>
     </row>
     <row r="194" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="9">
-        <v>14</v>
-      </c>
-      <c r="B194" s="24"/>
-      <c r="C194" s="24"/>
-      <c r="D194" s="24"/>
-      <c r="E194" s="24"/>
-      <c r="F194" s="24"/>
-      <c r="G194" s="24"/>
+        <v>192</v>
+      </c>
+      <c r="B194" s="26" t="s">
+        <v>770</v>
+      </c>
+      <c r="C194" s="24" t="s">
+        <v>806</v>
+      </c>
+      <c r="D194" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E194" s="24" t="s">
+        <v>800</v>
+      </c>
+      <c r="F194" s="24" t="s">
+        <v>791</v>
+      </c>
+      <c r="G194" s="24" t="s">
+        <v>779</v>
+      </c>
       <c r="H194" s="8"/>
     </row>
     <row r="195" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="9">
-        <v>14</v>
-      </c>
-      <c r="B195" s="24"/>
-      <c r="C195" s="24"/>
-      <c r="D195" s="24"/>
-      <c r="E195" s="24"/>
-      <c r="F195" s="24"/>
-      <c r="G195" s="24"/>
+        <v>193</v>
+      </c>
+      <c r="B195" s="26" t="s">
+        <v>770</v>
+      </c>
+      <c r="C195" s="24" t="s">
+        <v>807</v>
+      </c>
+      <c r="D195" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E195" s="24" t="s">
+        <v>799</v>
+      </c>
+      <c r="F195" s="24" t="s">
+        <v>792</v>
+      </c>
+      <c r="G195" s="24" t="s">
+        <v>780</v>
+      </c>
       <c r="H195" s="8"/>
     </row>
     <row r="196" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="9">
-        <v>14</v>
-      </c>
-      <c r="B196" s="24"/>
-      <c r="C196" s="24"/>
-      <c r="D196" s="24"/>
-      <c r="E196" s="24"/>
-      <c r="F196" s="24"/>
-      <c r="G196" s="24"/>
+        <v>194</v>
+      </c>
+      <c r="B196" s="26" t="s">
+        <v>770</v>
+      </c>
+      <c r="C196" s="24" t="s">
+        <v>808</v>
+      </c>
+      <c r="D196" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E196" s="24" t="s">
+        <v>798</v>
+      </c>
+      <c r="F196" s="24" t="s">
+        <v>793</v>
+      </c>
+      <c r="G196" s="24" t="s">
+        <v>781</v>
+      </c>
       <c r="H196" s="8"/>
     </row>
     <row r="197" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="9">
-        <v>14</v>
-      </c>
-      <c r="B197" s="24"/>
-      <c r="C197" s="24"/>
-      <c r="D197" s="24"/>
-      <c r="E197" s="24"/>
-      <c r="F197" s="24"/>
-      <c r="G197" s="24"/>
+        <v>195</v>
+      </c>
+      <c r="B197" s="26" t="s">
+        <v>770</v>
+      </c>
+      <c r="C197" s="24" t="s">
+        <v>809</v>
+      </c>
+      <c r="D197" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E197" s="24" t="s">
+        <v>797</v>
+      </c>
+      <c r="F197" s="24" t="s">
+        <v>794</v>
+      </c>
+      <c r="G197" s="24" t="s">
+        <v>782</v>
+      </c>
       <c r="H197" s="8"/>
     </row>
     <row r="198" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" s="9">
-        <v>14</v>
-      </c>
-      <c r="B198" s="24"/>
-      <c r="C198" s="24"/>
-      <c r="D198" s="24"/>
-      <c r="E198" s="24"/>
-      <c r="F198" s="24"/>
-      <c r="G198" s="24"/>
+        <v>196</v>
+      </c>
+      <c r="B198" s="26" t="s">
+        <v>770</v>
+      </c>
+      <c r="C198" s="24" t="s">
+        <v>810</v>
+      </c>
+      <c r="D198" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E198" s="24" t="s">
+        <v>796</v>
+      </c>
+      <c r="F198" s="24" t="s">
+        <v>795</v>
+      </c>
+      <c r="G198" s="24" t="s">
+        <v>783</v>
+      </c>
       <c r="H198" s="8"/>
     </row>
     <row r="199" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="9">
-        <v>14</v>
-      </c>
-      <c r="B199" s="24"/>
-      <c r="C199" s="24"/>
-      <c r="D199" s="24"/>
-      <c r="E199" s="24"/>
-      <c r="F199" s="24"/>
-      <c r="G199" s="24"/>
+        <v>197</v>
+      </c>
+      <c r="B199" s="26" t="s">
+        <v>770</v>
+      </c>
+      <c r="C199" s="24" t="s">
+        <v>811</v>
+      </c>
+      <c r="D199" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E199" s="24" t="s">
+        <v>819</v>
+      </c>
+      <c r="F199" s="24" t="s">
+        <v>823</v>
+      </c>
+      <c r="G199" s="24" t="s">
+        <v>825</v>
+      </c>
       <c r="H199" s="8"/>
     </row>
     <row r="200" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" s="9">
-        <v>14</v>
-      </c>
-      <c r="B200" s="24"/>
-      <c r="C200" s="24"/>
-      <c r="D200" s="24"/>
-      <c r="E200" s="24"/>
-      <c r="F200" s="24"/>
-      <c r="G200" s="24"/>
+        <v>198</v>
+      </c>
+      <c r="B200" s="26" t="s">
+        <v>770</v>
+      </c>
+      <c r="C200" s="24" t="s">
+        <v>812</v>
+      </c>
+      <c r="D200" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E200" s="24" t="s">
+        <v>822</v>
+      </c>
+      <c r="F200" s="24" t="s">
+        <v>824</v>
+      </c>
+      <c r="G200" s="24" t="s">
+        <v>826</v>
+      </c>
       <c r="H200" s="8"/>
     </row>
     <row r="201" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" s="9">
-        <v>14</v>
-      </c>
-      <c r="B201" s="24"/>
-      <c r="C201" s="24"/>
-      <c r="D201" s="24"/>
-      <c r="E201" s="24"/>
-      <c r="F201" s="24"/>
-      <c r="G201" s="24"/>
+        <v>199</v>
+      </c>
+      <c r="B201" s="26" t="s">
+        <v>770</v>
+      </c>
+      <c r="C201" s="24" t="s">
+        <v>813</v>
+      </c>
+      <c r="D201" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E201" s="24" t="s">
+        <v>829</v>
+      </c>
+      <c r="F201" s="24" t="s">
+        <v>850</v>
+      </c>
+      <c r="G201" s="24" t="s">
+        <v>827</v>
+      </c>
       <c r="H201" s="8"/>
     </row>
     <row r="202" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" s="9">
-        <v>14</v>
-      </c>
-      <c r="B202" s="24"/>
-      <c r="C202" s="24"/>
-      <c r="D202" s="24"/>
-      <c r="E202" s="24"/>
-      <c r="F202" s="24"/>
-      <c r="G202" s="24"/>
+        <v>200</v>
+      </c>
+      <c r="B202" s="26" t="s">
+        <v>770</v>
+      </c>
+      <c r="C202" s="24" t="s">
+        <v>814</v>
+      </c>
+      <c r="D202" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E202" s="24" t="s">
+        <v>830</v>
+      </c>
+      <c r="F202" s="24" t="s">
+        <v>851</v>
+      </c>
+      <c r="G202" s="24" t="s">
+        <v>828</v>
+      </c>
       <c r="H202" s="8"/>
     </row>
     <row r="203" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A203" s="9">
-        <v>14</v>
-      </c>
-      <c r="B203" s="24"/>
-      <c r="C203" s="24"/>
-      <c r="D203" s="24"/>
-      <c r="E203" s="24"/>
-      <c r="F203" s="24"/>
-      <c r="G203" s="24"/>
+        <v>201</v>
+      </c>
+      <c r="B203" s="24" t="s">
+        <v>815</v>
+      </c>
+      <c r="C203" s="24" t="s">
+        <v>817</v>
+      </c>
+      <c r="D203" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E203" s="24" t="s">
+        <v>760</v>
+      </c>
+      <c r="F203" s="24" t="s">
+        <v>852</v>
+      </c>
+      <c r="G203" s="24" t="s">
+        <v>857</v>
+      </c>
       <c r="H203" s="8"/>
     </row>
     <row r="204" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="9">
-        <v>14</v>
-      </c>
-      <c r="B204" s="24"/>
-      <c r="C204" s="24"/>
-      <c r="D204" s="24"/>
-      <c r="E204" s="24"/>
-      <c r="F204" s="24"/>
-      <c r="G204" s="24"/>
+        <v>202</v>
+      </c>
+      <c r="B204" s="24" t="s">
+        <v>816</v>
+      </c>
+      <c r="C204" s="24" t="s">
+        <v>818</v>
+      </c>
+      <c r="D204" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E204" s="24" t="s">
+        <v>831</v>
+      </c>
+      <c r="F204" s="24" t="s">
+        <v>853</v>
+      </c>
+      <c r="G204" s="26" t="s">
+        <v>863</v>
+      </c>
       <c r="H204" s="8"/>
     </row>
     <row r="205" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" s="9">
-        <v>14</v>
-      </c>
-      <c r="B205" s="25"/>
-      <c r="C205" s="25"/>
-      <c r="D205" s="25"/>
-      <c r="E205" s="25"/>
-      <c r="F205" s="25"/>
-      <c r="G205" s="25"/>
+        <v>203</v>
+      </c>
+      <c r="B205" s="25" t="s">
+        <v>820</v>
+      </c>
+      <c r="C205" s="25" t="s">
+        <v>821</v>
+      </c>
+      <c r="D205" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E205" s="25" t="s">
+        <v>832</v>
+      </c>
+      <c r="F205" s="25" t="s">
+        <v>854</v>
+      </c>
+      <c r="G205" s="25" t="s">
+        <v>864</v>
+      </c>
       <c r="H205" s="8"/>
     </row>
     <row r="206" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" s="9">
-        <v>14</v>
-      </c>
-      <c r="B206" s="25"/>
-      <c r="C206" s="25"/>
-      <c r="D206" s="25"/>
-      <c r="E206" s="25"/>
-      <c r="F206" s="25"/>
-      <c r="G206" s="25"/>
+        <v>204</v>
+      </c>
+      <c r="B206" s="25" t="s">
+        <v>820</v>
+      </c>
+      <c r="C206" s="25" t="s">
+        <v>836</v>
+      </c>
+      <c r="D206" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E206" s="25" t="s">
+        <v>833</v>
+      </c>
+      <c r="F206" s="25" t="s">
+        <v>855</v>
+      </c>
+      <c r="G206" s="25" t="s">
+        <v>865</v>
+      </c>
       <c r="H206" s="8"/>
     </row>
     <row r="207" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" s="9">
-        <v>14</v>
-      </c>
-      <c r="B207" s="25"/>
-      <c r="C207" s="25"/>
-      <c r="D207" s="25"/>
-      <c r="E207" s="25"/>
-      <c r="F207" s="25"/>
-      <c r="G207" s="25"/>
+        <v>205</v>
+      </c>
+      <c r="B207" s="25" t="s">
+        <v>820</v>
+      </c>
+      <c r="C207" s="25" t="s">
+        <v>837</v>
+      </c>
+      <c r="D207" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E207" s="25" t="s">
+        <v>834</v>
+      </c>
+      <c r="F207" s="25" t="s">
+        <v>856</v>
+      </c>
+      <c r="G207" s="25" t="s">
+        <v>858</v>
+      </c>
       <c r="H207" s="8"/>
     </row>
     <row r="208" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A208" s="9">
-        <v>14</v>
-      </c>
-      <c r="B208" s="25"/>
-      <c r="C208" s="25"/>
-      <c r="D208" s="25"/>
-      <c r="E208" s="25"/>
-      <c r="F208" s="25"/>
-      <c r="G208" s="25"/>
+        <v>206</v>
+      </c>
+      <c r="B208" s="25" t="s">
+        <v>820</v>
+      </c>
+      <c r="C208" s="25" t="s">
+        <v>838</v>
+      </c>
+      <c r="D208" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E208" s="25" t="s">
+        <v>835</v>
+      </c>
+      <c r="F208" s="25" t="s">
+        <v>856</v>
+      </c>
+      <c r="G208" s="25" t="s">
+        <v>859</v>
+      </c>
       <c r="H208" s="8"/>
     </row>
     <row r="209" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" s="9">
-        <v>14</v>
-      </c>
-      <c r="B209" s="25"/>
-      <c r="C209" s="25"/>
-      <c r="D209" s="25"/>
-      <c r="E209" s="25"/>
-      <c r="F209" s="25"/>
-      <c r="G209" s="25"/>
+        <v>207</v>
+      </c>
+      <c r="B209" s="25" t="s">
+        <v>820</v>
+      </c>
+      <c r="C209" s="25" t="s">
+        <v>839</v>
+      </c>
+      <c r="D209" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E209" s="25" t="s">
+        <v>874</v>
+      </c>
+      <c r="F209" s="25" t="s">
+        <v>885</v>
+      </c>
+      <c r="G209" s="25" t="s">
+        <v>860</v>
+      </c>
       <c r="H209" s="8"/>
     </row>
     <row r="210" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" s="9">
-        <v>14</v>
-      </c>
-      <c r="B210" s="25"/>
-      <c r="C210" s="25"/>
-      <c r="D210" s="25"/>
-      <c r="E210" s="25"/>
-      <c r="F210" s="25"/>
-      <c r="G210" s="25"/>
+        <v>208</v>
+      </c>
+      <c r="B210" s="25" t="s">
+        <v>820</v>
+      </c>
+      <c r="C210" s="25" t="s">
+        <v>840</v>
+      </c>
+      <c r="D210" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E210" s="25" t="s">
+        <v>875</v>
+      </c>
+      <c r="F210" s="25" t="s">
+        <v>886</v>
+      </c>
+      <c r="G210" s="25" t="s">
+        <v>861</v>
+      </c>
       <c r="H210" s="8"/>
     </row>
     <row r="211" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="9">
-        <v>14</v>
-      </c>
-      <c r="B211" s="25"/>
-      <c r="C211" s="25"/>
-      <c r="D211" s="25"/>
-      <c r="E211" s="25"/>
-      <c r="F211" s="25"/>
-      <c r="G211" s="25"/>
+        <v>209</v>
+      </c>
+      <c r="B211" s="25" t="s">
+        <v>820</v>
+      </c>
+      <c r="C211" s="25" t="s">
+        <v>841</v>
+      </c>
+      <c r="D211" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E211" s="25" t="s">
+        <v>876</v>
+      </c>
+      <c r="F211" s="25" t="s">
+        <v>887</v>
+      </c>
+      <c r="G211" s="25" t="s">
+        <v>862</v>
+      </c>
       <c r="H211" s="8"/>
     </row>
     <row r="212" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="9">
-        <v>14</v>
-      </c>
-      <c r="B212" s="25"/>
-      <c r="C212" s="25"/>
-      <c r="D212" s="25"/>
-      <c r="E212" s="25"/>
-      <c r="F212" s="25"/>
-      <c r="G212" s="25"/>
+        <v>210</v>
+      </c>
+      <c r="B212" s="25" t="s">
+        <v>820</v>
+      </c>
+      <c r="C212" s="25" t="s">
+        <v>842</v>
+      </c>
+      <c r="D212" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E212" s="25" t="s">
+        <v>877</v>
+      </c>
+      <c r="F212" s="25" t="s">
+        <v>888</v>
+      </c>
+      <c r="G212" s="25" t="s">
+        <v>866</v>
+      </c>
       <c r="H212" s="8"/>
     </row>
     <row r="213" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A213" s="9">
-        <v>14</v>
-      </c>
-      <c r="B213" s="25"/>
-      <c r="C213" s="25"/>
-      <c r="D213" s="25"/>
-      <c r="E213" s="25"/>
-      <c r="F213" s="25"/>
-      <c r="G213" s="25"/>
+        <v>211</v>
+      </c>
+      <c r="B213" s="25" t="s">
+        <v>820</v>
+      </c>
+      <c r="C213" s="25" t="s">
+        <v>843</v>
+      </c>
+      <c r="D213" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E213" s="25" t="s">
+        <v>878</v>
+      </c>
+      <c r="F213" s="25" t="s">
+        <v>889</v>
+      </c>
+      <c r="G213" s="25" t="s">
+        <v>867</v>
+      </c>
       <c r="H213" s="8"/>
     </row>
     <row r="214" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="9">
-        <v>14</v>
-      </c>
-      <c r="B214" s="25"/>
-      <c r="C214" s="25"/>
-      <c r="D214" s="25"/>
-      <c r="E214" s="25"/>
-      <c r="F214" s="25"/>
-      <c r="G214" s="25"/>
+        <v>212</v>
+      </c>
+      <c r="B214" s="25" t="s">
+        <v>820</v>
+      </c>
+      <c r="C214" s="25" t="s">
+        <v>844</v>
+      </c>
+      <c r="D214" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E214" s="25" t="s">
+        <v>879</v>
+      </c>
+      <c r="F214" s="25" t="s">
+        <v>890</v>
+      </c>
+      <c r="G214" s="25" t="s">
+        <v>868</v>
+      </c>
       <c r="H214" s="8"/>
     </row>
     <row r="215" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="9">
-        <v>14</v>
-      </c>
-      <c r="B215" s="25"/>
-      <c r="C215" s="25"/>
-      <c r="D215" s="25"/>
-      <c r="E215" s="25"/>
+        <v>213</v>
+      </c>
+      <c r="B215" s="25" t="s">
+        <v>820</v>
+      </c>
+      <c r="C215" s="25" t="s">
+        <v>845</v>
+      </c>
+      <c r="D215" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E215" s="25" t="s">
+        <v>880</v>
+      </c>
       <c r="F215" s="25"/>
-      <c r="G215" s="25"/>
+      <c r="G215" s="25" t="s">
+        <v>869</v>
+      </c>
       <c r="H215" s="8"/>
     </row>
     <row r="216" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A216" s="9">
-        <v>14</v>
-      </c>
-      <c r="B216" s="25"/>
-      <c r="C216" s="25"/>
-      <c r="D216" s="25"/>
-      <c r="E216" s="25"/>
+        <v>214</v>
+      </c>
+      <c r="B216" s="25" t="s">
+        <v>820</v>
+      </c>
+      <c r="C216" s="25" t="s">
+        <v>846</v>
+      </c>
+      <c r="D216" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E216" s="25" t="s">
+        <v>881</v>
+      </c>
       <c r="F216" s="25"/>
-      <c r="G216" s="25"/>
+      <c r="G216" s="25" t="s">
+        <v>870</v>
+      </c>
       <c r="H216" s="8"/>
     </row>
     <row r="217" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A217" s="9">
-        <v>14</v>
-      </c>
-      <c r="B217" s="25"/>
-      <c r="C217" s="25"/>
-      <c r="D217" s="25"/>
-      <c r="E217" s="25"/>
+        <v>215</v>
+      </c>
+      <c r="B217" s="25" t="s">
+        <v>820</v>
+      </c>
+      <c r="C217" s="25" t="s">
+        <v>847</v>
+      </c>
+      <c r="D217" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E217" s="25" t="s">
+        <v>882</v>
+      </c>
       <c r="F217" s="25"/>
-      <c r="G217" s="25"/>
+      <c r="G217" s="25" t="s">
+        <v>871</v>
+      </c>
       <c r="H217" s="8"/>
     </row>
     <row r="218" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" s="9">
-        <v>14</v>
-      </c>
-      <c r="B218" s="13"/>
-      <c r="C218" s="13"/>
-      <c r="D218" s="13"/>
-      <c r="E218" s="13"/>
+        <v>216</v>
+      </c>
+      <c r="B218" s="25" t="s">
+        <v>820</v>
+      </c>
+      <c r="C218" s="13" t="s">
+        <v>848</v>
+      </c>
+      <c r="D218" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E218" s="13" t="s">
+        <v>883</v>
+      </c>
       <c r="F218" s="13"/>
-      <c r="G218" s="13"/>
+      <c r="G218" s="25" t="s">
+        <v>872</v>
+      </c>
       <c r="H218" s="8"/>
     </row>
     <row r="219" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="9">
-        <v>14</v>
-      </c>
-      <c r="B219" s="13"/>
-      <c r="C219" s="13"/>
-      <c r="D219" s="13"/>
-      <c r="E219" s="13"/>
+        <v>217</v>
+      </c>
+      <c r="B219" s="25" t="s">
+        <v>820</v>
+      </c>
+      <c r="C219" s="13" t="s">
+        <v>849</v>
+      </c>
+      <c r="D219" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E219" s="13" t="s">
+        <v>884</v>
+      </c>
       <c r="F219" s="13"/>
-      <c r="G219" s="13"/>
+      <c r="G219" s="25" t="s">
+        <v>873</v>
+      </c>
       <c r="H219" s="8"/>
     </row>
     <row r="220" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" s="9">
-        <v>14</v>
+        <v>218</v>
       </c>
       <c r="B220" s="13"/>
       <c r="C220" s="13"/>
       <c r="D220" s="13"/>
       <c r="E220" s="13"/>
       <c r="F220" s="13"/>
-      <c r="G220" s="13"/>
+      <c r="G220" s="25"/>
       <c r="H220" s="8"/>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A221" s="9">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A222" s="31">
+        <v>220</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>